<commit_message>
feat: sjablonen  nieuwe kolommen: Toelichting, soorten-bewijs met vinkjes (multi), koppeling aan Portfolio/cursus; delimiter ; of ,; EVL 1,21.2; filtering sjablonen per gekozen cursus
</commit_message>
<xml_diff>
--- a/public/Sjablonen/25-26-Sjablonen.xlsx
+++ b/public/Sjablonen/25-26-Sjablonen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Jouw Portfolio plan\public\Sjablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98872905-3A4C-4665-9C26-88224E0AC496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048EA695-3576-4A75-A4A5-48605288B64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="44">
   <si>
     <t>Naam</t>
   </si>
@@ -41,9 +41,6 @@
     <t>EVL</t>
   </si>
   <si>
-    <t>Casussen</t>
-  </si>
-  <si>
     <t>Kennis</t>
   </si>
   <si>
@@ -62,27 +59,15 @@
     <t>Kwantiteit</t>
   </si>
   <si>
-    <t>Soort</t>
-  </si>
-  <si>
     <t>Voorbeeld sjabloon</t>
   </si>
   <si>
-    <t>1.1, 1.2</t>
-  </si>
-  <si>
     <t>Anatomie</t>
   </si>
   <si>
-    <t>document</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
-    <t>Behandelplan</t>
-  </si>
-  <si>
     <t>Return2Performande</t>
   </si>
   <si>
@@ -113,7 +98,73 @@
     <t>Portfolio</t>
   </si>
   <si>
-    <t>Anamnese simulatie</t>
+    <t>Toelichting</t>
+  </si>
+  <si>
+    <t>Schriftelijk product</t>
+  </si>
+  <si>
+    <t>1.1; 1.2</t>
+  </si>
+  <si>
+    <t>Soort Bewijs</t>
+  </si>
+  <si>
+    <t>Certificaat</t>
+  </si>
+  <si>
+    <t>Kennistoets</t>
+  </si>
+  <si>
+    <t>Vaardigheidstest</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Gesprek</t>
+  </si>
+  <si>
+    <t>Overig</t>
+  </si>
+  <si>
+    <t>Dit is slechts een voorbeeld</t>
+  </si>
+  <si>
+    <t>Behandelplan Uitvoeren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uitvoeren anamnese </t>
+  </si>
+  <si>
+    <t>Je voert een anamnese uit bij een (simulatie) patient. Een simulatiepatient kan bijvoorbeeld een medestudent, docent, acteur, AI chatbot zijn.</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>Behandelplan opstellen</t>
+  </si>
+  <si>
+    <t>dit is een test</t>
+  </si>
+  <si>
+    <t>Feedbackmoment kennis ZONDER surveillanten</t>
+  </si>
+  <si>
+    <t>Feedbackmoment kennis MET surveillanten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LVT (Landelijke voortgangstoets) </t>
+  </si>
+  <si>
+    <t>e-learning 'AI basiskennis en vaardigheden'</t>
+  </si>
+  <si>
+    <t>Anatomie; Pathofysiologie; Gedrag &amp; Communicatie; Vak Fysiotherapie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,1; 4.3; </t>
   </si>
 </sst>
 </file>
@@ -129,12 +180,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,9 +206,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -491,175 +556,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="26.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="20" width="5.5" customWidth="1"/>
+    <col min="1" max="2" width="26.59765625" style="1"/>
+    <col min="3" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" style="3" customWidth="1"/>
+    <col min="11" max="17" width="7.69921875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.59765625" style="3" customWidth="1"/>
+    <col min="19" max="27" width="5.59765625" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="26.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:27" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>24</v>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" t="s">
-        <v>14</v>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+    <row r="4" spans="1:27" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" t="s">
-        <v>14</v>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>26</v>
+    <row r="5" spans="1:27" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J1 A2:B2 D2:J2" numberStoredAsText="1"/>
+    <ignoredError sqref="C1 D2:I2 A2 A1 D1:I1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ui(matrix): toon individuele tegels voor casussen en kennis (zelfde stijl als EVL) i.p.v. tellers
</commit_message>
<xml_diff>
--- a/public/Sjablonen/25-26-Sjablonen.xlsx
+++ b/public/Sjablonen/25-26-Sjablonen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Jouw Portfolio plan\public\Sjablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048EA695-3576-4A75-A4A5-48605288B64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7E9230-402C-4079-9730-D8BA2715FF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
   <si>
     <t>Naam</t>
   </si>
@@ -68,9 +68,6 @@
     <t>v</t>
   </si>
   <si>
-    <t>Return2Performande</t>
-  </si>
-  <si>
     <t>Fit in the Hood</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t xml:space="preserve">4,1; 4.3; </t>
+  </si>
+  <si>
+    <t>Return2Performance</t>
   </si>
 </sst>
 </file>
@@ -559,20 +559,36 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="26.59765625" style="1"/>
-    <col min="3" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.59765625" style="3" customWidth="1"/>
-    <col min="11" max="17" width="7.69921875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.59765625" style="3" customWidth="1"/>
-    <col min="19" max="27" width="5.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.69921875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.69921875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.59765625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="5.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="5.59765625" style="1" customWidth="1"/>
+    <col min="24" max="25" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="5.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="16384" width="26.59765625" style="1"/>
   </cols>
   <sheetData>
@@ -581,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -605,58 +621,58 @@
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="R1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
@@ -664,10 +680,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -720,16 +736,19 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="1">
         <v>2.1</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>10</v>
@@ -761,13 +780,13 @@
     </row>
     <row r="4" spans="1:27" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -781,7 +800,7 @@
       <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -814,10 +833,10 @@
     </row>
     <row r="5" spans="1:27" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C5" s="1">
         <v>1.1000000000000001</v>
@@ -867,10 +886,10 @@
     </row>
     <row r="6" spans="1:27" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>10</v>
@@ -902,10 +921,10 @@
     </row>
     <row r="7" spans="1:27" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>10</v>
@@ -937,10 +956,10 @@
     </row>
     <row r="8" spans="1:27" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>10</v>
@@ -972,10 +991,10 @@
     </row>
     <row r="9" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>10</v>

</xml_diff>